<commit_message>
Added 0.15.0 test publication
</commit_message>
<xml_diff>
--- a/Webroot/core/CodeSystem-city-symbol.xlsx
+++ b/Webroot/core/CodeSystem-city-symbol.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.14.0</t>
+    <t>0.15.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-12-05T11:14:13+01:00</t>
+    <t>2023-12-21T10:19:00+01:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>